<commit_message>
Final push for week 2
</commit_message>
<xml_diff>
--- a/Planning and Design/Sprint Product Log.xlsx
+++ b/Planning and Design/Sprint Product Log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\CST-247\Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\CST-247\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14FB9F-CC14-4458-BDA8-0D532F6D31A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1936E73D-2030-4098-A6AE-9BFAB3117CF0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Project Title:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>User Stories</t>
   </si>
@@ -60,22 +57,38 @@
     <t>Modification Date</t>
   </si>
   <si>
-    <t>Create Backlog</t>
+    <t>Webpage</t>
   </si>
   <si>
-    <t>Team Meeting</t>
+    <t>Login Feature</t>
   </si>
   <si>
-    <t>Team is on the same page</t>
+    <t>Registration</t>
   </si>
   <si>
-    <t>Team understands what to do</t>
+    <t>Allow registered users to login</t>
   </si>
   <si>
-    <t xml:space="preserve">Documentation </t>
+    <t>Register new users</t>
   </si>
   <si>
-    <t>Everything is recorded</t>
+    <t>they can play the game</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Refactor existing code</t>
+  </si>
+  <si>
+    <t>make exisitng code neater
+ and remove redundant code</t>
+  </si>
+  <si>
+    <t>Project Title: Minesweeper Version 1.1</t>
   </si>
 </sst>
 </file>
@@ -243,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -278,6 +291,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,8 +306,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2060"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,14 +609,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
+      <c r="A1" s="21" t="s">
+        <v>20</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -609,105 +625,123 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="16" t="s">
-        <v>1</v>
+      <c r="D2" s="18" t="s">
+        <v>0</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="5"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="15"/>
+      <c r="C4" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" s="10"/>
       <c r="E4" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="14">
         <v>1</v>
       </c>
-      <c r="H4" s="21">
-        <v>43345</v>
+      <c r="H4" s="16">
+        <v>43346</v>
       </c>
-      <c r="I4" s="22">
-        <v>43345</v>
+      <c r="I4" s="17">
+        <v>43351</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="15"/>
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="D5" s="10"/>
       <c r="E5" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" s="14">
         <v>1</v>
       </c>
-      <c r="H5" s="21">
-        <v>43345</v>
+      <c r="H5" s="16">
+        <v>43346</v>
       </c>
-      <c r="I5" s="22">
-        <v>43345</v>
+      <c r="I5" s="17">
+        <v>43351</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="15"/>
+    <row r="6" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="D6" s="10"/>
       <c r="E6" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>16</v>
+      <c r="F6" s="23" t="s">
+        <v>19</v>
       </c>
       <c r="G6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
-      <c r="H6" s="21">
-        <v>43345</v>
+      <c r="H6" s="16">
+        <v>43346</v>
       </c>
-      <c r="I6" s="22">
-        <v>43345</v>
+      <c r="I6" s="17">
+        <v>43347</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -23318,6 +23352,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
@@ -23370,31 +23413,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>False</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Course Development" ma:contentTypeID="0x010100A30BC5E90BED914E81F4B67CDEADBEEF0072B4D5296E9CCD41A4B955E8BC4A98B900B6D41DF35BCF664B888FA24C3105B583" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new Course Development document." ma:contentTypeScope="" ma:versionID="9dd9ed6e3bbe7b4f5b00c4ab3cb49488">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="30a82cfc-8d0b-455e-b705-4035c60ff9fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f302115a5f8a1b15560b600ae7cd187" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -23623,7 +23642,30 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>False</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A856C235-C1E3-486A-AF6F-91B1EB05F3BD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -23640,31 +23682,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1713361C-F80E-4293-9FB3-5DC100B81DE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{543DFEB0-7AA3-434C-B1C2-BCF78AB39365}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68741204-811B-4110-9B64-9D55504528C5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23681,4 +23699,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{543DFEB0-7AA3-434C-B1C2-BCF78AB39365}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1713361C-F80E-4293-9FB3-5DC100B81DE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>